<commit_message>
Working effects: spiral, pulse, firefly, spinning.
</commit_message>
<xml_diff>
--- a/color numbering.xlsx
+++ b/color numbering.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="210" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="210" windowWidth="20115" windowHeight="7935" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Color map" sheetId="1" r:id="rId1"/>
+    <sheet name="Spiral" sheetId="2" r:id="rId2"/>
+    <sheet name="Spinning" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>R</t>
   </si>
@@ -34,6 +35,30 @@
   </si>
   <si>
     <t>Pixel</t>
+  </si>
+  <si>
+    <t>Spin</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>1/6</t>
+  </si>
+  <si>
+    <t>2/6</t>
+  </si>
+  <si>
+    <t>3/6</t>
+  </si>
+  <si>
+    <t>4/6</t>
+  </si>
+  <si>
+    <t>5/6</t>
+  </si>
+  <si>
+    <t>6/6</t>
   </si>
 </sst>
 </file>
@@ -69,8 +94,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -110,7 +136,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>'Color map'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -124,7 +150,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:f>'Color map'!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -159,7 +185,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>'Color map'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -173,7 +199,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:f>'Color map'!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -208,7 +234,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>'Color map'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -222,7 +248,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:f>'Color map'!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -262,11 +288,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="41073664"/>
-        <c:axId val="41075456"/>
+        <c:axId val="98428032"/>
+        <c:axId val="98429568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="41073664"/>
+        <c:axId val="98428032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -275,7 +301,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41075456"/>
+        <c:crossAx val="98429568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -283,7 +309,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41075456"/>
+        <c:axId val="98429568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -294,7 +320,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41073664"/>
+        <c:crossAx val="98428032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -640,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,10 +789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="I12" sqref="I1:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,7 +800,7 @@
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -791,288 +817,320 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>120</v>
+        <v>255</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>255</v>
+        <v>170</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G36" si="0">C2&amp;","&amp;D2&amp;","&amp;E2&amp;","</f>
-        <v>120,0,255,</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>255,0,170,</v>
+      </c>
+      <c r="I2">
+        <f>2*PI()/7*(A2-1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>130</v>
+        <v>255</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>255</v>
+        <v>180</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
-        <v>130,0,255,</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>255,0,180,</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I9" si="1">2*PI()/8*(A3-1)</f>
+        <v>0.78539816339744828</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>255</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>190</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>255,0,190,</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>1.5707963267948966</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>255</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>200</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>255,0,200,</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>2.3561944901923448</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>255</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>210</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>255,0,210,</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>255</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>220</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>255,0,220,</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>3.9269908169872414</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>255</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>230</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>255,0,230,</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>4.7123889803846897</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>255</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>240</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>255,0,240,</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>5.497787143782138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>255</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>250</v>
+      </c>
+      <c r="G10" t="str">
+        <f>C10&amp;","&amp;D10&amp;","&amp;E10&amp;","</f>
+        <v>255,0,250,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B11">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C11">
         <v>250</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>255</v>
-      </c>
-      <c r="G4" t="str">
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>255</v>
+      </c>
+      <c r="G11" t="str">
         <f t="shared" si="0"/>
         <v>250,0,255,</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>24</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>110</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>255</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" si="0"/>
-        <v>110,0,255,</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>25</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>255</v>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" si="0"/>
-        <v>100,0,255,</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B12">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C12">
         <v>240</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>255</v>
-      </c>
-      <c r="G7" t="str">
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>255</v>
+      </c>
+      <c r="G12" t="str">
         <f t="shared" si="0"/>
         <v>240,0,255,</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>255</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>170</v>
-      </c>
-      <c r="G8" t="str">
-        <f t="shared" si="0"/>
-        <v>255,0,170,</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>255</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>250</v>
-      </c>
-      <c r="G9" t="str">
-        <f t="shared" si="0"/>
-        <v>255,0,250,</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>21</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>140</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>255</v>
-      </c>
-      <c r="G10" t="str">
-        <f t="shared" si="0"/>
-        <v>140,0,255,</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>35</v>
-      </c>
-      <c r="B11">
-        <v>9</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>255</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="0"/>
-        <v>0,0,255,</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>20</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>150</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>255</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="0"/>
-        <v>150,0,255,</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C13">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>255,0,240,</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>230,0,255,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C14">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>180</v>
+        <v>255</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>255,0,180,</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>220,0,255,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C15">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1082,18 +1140,18 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>230,0,255,</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>210,0,255,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C16">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1103,18 +1161,18 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>90,0,255,</v>
+        <v>200,0,255,</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
         <v>27</v>
       </c>
-      <c r="B17">
-        <v>15</v>
-      </c>
       <c r="C17">
-        <v>80</v>
+        <v>190</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1124,18 +1182,18 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>80,0,255,</v>
+        <v>190,0,255,</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C18">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1145,123 +1203,123 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>220,0,255,</v>
+        <v>180,0,255,</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C19">
-        <v>255</v>
+        <v>170</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>190</v>
+        <v>255</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>255,0,190,</v>
+        <v>170,0,255,</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C20">
-        <v>255</v>
+        <v>160</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>200</v>
+        <v>255</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>255,0,200,</v>
+        <v>160,0,255,</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>255</v>
+        <v>150</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>210</v>
+        <v>255</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>255,0,210,</v>
+        <v>150,0,255,</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>255</v>
+        <v>140</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>255,0,220,</v>
+        <v>140,0,255,</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>255</v>
+        <v>130</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>230</v>
+        <v>255</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>255,0,230,</v>
+        <v>130,0,255,</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1271,18 +1329,18 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>160,0,255,</v>
+        <v>120,0,255,</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C25">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1292,18 +1350,18 @@
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>10,0,255,</v>
+        <v>110,0,255,</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C26">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1313,18 +1371,18 @@
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>20,0,255,</v>
+        <v>100,0,255,</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C27">
-        <v>170</v>
+        <v>90</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -1334,18 +1392,18 @@
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>170,0,255,</v>
+        <v>90,0,255,</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>180</v>
+        <v>80</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -1355,18 +1413,18 @@
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>180,0,255,</v>
+        <v>80,0,255,</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C29">
-        <v>190</v>
+        <v>70</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1376,18 +1434,18 @@
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>190,0,255,</v>
+        <v>70,0,255,</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C30">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -1397,18 +1455,18 @@
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>200,0,255,</v>
+        <v>60,0,255,</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B31">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C31">
-        <v>210</v>
+        <v>50</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1418,18 +1476,18 @@
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>210,0,255,</v>
+        <v>50,0,255,</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B32">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C32">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1439,18 +1497,18 @@
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>70,0,255,</v>
+        <v>40,0,255,</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B33">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C33">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1460,18 +1518,18 @@
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v>60,0,255,</v>
+        <v>30,0,255,</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B34">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C34">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1481,18 +1539,18 @@
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
-        <v>50,0,255,</v>
+        <v>20,0,255,</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B35">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C35">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1502,18 +1560,18 @@
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
-        <v>40,0,255,</v>
+        <v>10,0,255,</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B36">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="C36">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1523,18 +1581,1435 @@
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
-        <v>30,0,255,</v>
+        <v>0,0,255,</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:E36">
-    <sortCondition ref="B2:B36"/>
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="D2" t="str">
+        <f>IF(A2/$K2 &lt; 1/6,E2,IF(A2/$K2&lt;2/6,F2,IF(A2/$K2&lt;3/6,G2,IF(A2/$K2&lt;4/6,H2,IF(A2/$K2&lt;5/6,I2,J2)))))</f>
+        <v>0,0,255,</v>
+      </c>
+      <c r="E2" t="str">
+        <f>ROUND(A2/$K2*255,0)&amp;",0,255,"</f>
+        <v>0,0,255,</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"255,0,"&amp;ROUND(($K2-A2)/$K2*255,0)&amp;","</f>
+        <v>255,0,255,</v>
+      </c>
+      <c r="G2" t="str">
+        <f>"255,"&amp;ROUND(A2/$K2*255,0)&amp;",0,"</f>
+        <v>255,0,0,</v>
+      </c>
+      <c r="H2" t="str">
+        <f>ROUND(($K2-A2)/$K2*255,0)&amp;",255,0,"</f>
+        <v>255,255,0,</v>
+      </c>
+      <c r="I2" t="str">
+        <f>"0,255,"&amp;ROUND(A2/$K2*255,0)&amp;","</f>
+        <v>0,255,0,</v>
+      </c>
+      <c r="J2" t="str">
+        <f>"0,"&amp;ROUND(($K2-A2)/$K2*255,0)&amp;",255,"</f>
+        <v>0,255,255,</v>
+      </c>
+      <c r="K2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D9" si="0">IF(A3/$K3 &lt; 1/6,E3,IF(A3/$K3&lt;2/6,F3,IF(A3/$K3&lt;3/6,G3,IF(A3/$K3&lt;4/6,H3,IF(A3/$K3&lt;5/6,I3,J3)))))</f>
+        <v>32,0,255,</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E9" si="1">ROUND(A3/$K3*255,0)&amp;",0,255,"</f>
+        <v>32,0,255,</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F9" si="2">"255,0,"&amp;ROUND(($K3-A3)/$K3*255,0)&amp;","</f>
+        <v>255,0,223,</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G9" si="3">"255,"&amp;ROUND(A3/$K3*255,0)&amp;",0,"</f>
+        <v>255,32,0,</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H9" si="4">ROUND(($K3-A3)/$K3*255,0)&amp;",255,0,"</f>
+        <v>223,255,0,</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I9" si="5">"0,255,"&amp;ROUND(A3/$K3*255,0)&amp;","</f>
+        <v>0,255,32,</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J9" si="6">"0,"&amp;ROUND(($K3-A3)/$K3*255,0)&amp;",255,"</f>
+        <v>0,223,255,</v>
+      </c>
+      <c r="K3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>255,0,191,</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>64,0,255,</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="2"/>
+        <v>255,0,191,</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="3"/>
+        <v>255,64,0,</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="4"/>
+        <v>191,255,0,</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="5"/>
+        <v>0,255,64,</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="6"/>
+        <v>0,191,255,</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>18</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>255,96,0,</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>96,0,255,</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="2"/>
+        <v>255,0,159,</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="3"/>
+        <v>255,96,0,</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="4"/>
+        <v>159,255,0,</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="5"/>
+        <v>0,255,96,</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="6"/>
+        <v>0,159,255,</v>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>19</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>128,255,0,</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>128,0,255,</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="2"/>
+        <v>255,0,128,</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="3"/>
+        <v>255,128,0,</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="4"/>
+        <v>128,255,0,</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="5"/>
+        <v>0,255,128,</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="6"/>
+        <v>0,128,255,</v>
+      </c>
+      <c r="K6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>96,255,0,</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>159,0,255,</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="2"/>
+        <v>255,0,96,</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="3"/>
+        <v>255,159,0,</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="4"/>
+        <v>96,255,0,</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="5"/>
+        <v>0,255,159,</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="6"/>
+        <v>0,96,255,</v>
+      </c>
+      <c r="K7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>21</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>0,255,191,</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>191,0,255,</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="2"/>
+        <v>255,0,64,</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="3"/>
+        <v>255,191,0,</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="4"/>
+        <v>64,255,0,</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="5"/>
+        <v>0,255,191,</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="6"/>
+        <v>0,64,255,</v>
+      </c>
+      <c r="K8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>0,32,255,</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>223,0,255,</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="2"/>
+        <v>255,0,32,</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="3"/>
+        <v>255,223,0,</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="4"/>
+        <v>32,255,0,</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="5"/>
+        <v>0,255,223,</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="6"/>
+        <v>0,32,255,</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" ref="D10:D36" si="7">IF(A10/$K10 &lt; 1/6,E10,IF(A10/$K10&lt;2/6,F10,IF(A10/$K10&lt;3/6,G10,IF(A10/$K10&lt;4/6,H10,IF(A10/$K10&lt;5/6,I10,J10)))))</f>
+        <v>0,0,255,</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" ref="E10:E36" si="8">ROUND(A10/$K10*255,0)&amp;",0,255,"</f>
+        <v>0,0,255,</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" ref="F10:F36" si="9">"255,0,"&amp;ROUND(($K10-A10)/$K10*255,0)&amp;","</f>
+        <v>255,0,255,</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" ref="G10:G36" si="10">"255,"&amp;ROUND(A10/$K10*255,0)&amp;",0,"</f>
+        <v>255,0,0,</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" ref="H10:H36" si="11">ROUND(($K10-A10)/$K10*255,0)&amp;",255,0,"</f>
+        <v>255,255,0,</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" ref="I10:I36" si="12">"0,255,"&amp;ROUND(A10/$K10*255,0)&amp;","</f>
+        <v>0,255,0,</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" ref="J10:J36" si="13">"0,"&amp;ROUND(($K10-A10)/$K10*255,0)&amp;",255,"</f>
+        <v>0,255,255,</v>
+      </c>
+      <c r="K10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="7"/>
+        <v>21,0,255,</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="8"/>
+        <v>21,0,255,</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,234,</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="10"/>
+        <v>255,21,0,</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="11"/>
+        <v>234,255,0,</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,21,</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="13"/>
+        <v>0,234,255,</v>
+      </c>
+      <c r="K11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>13</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="7"/>
+        <v>255,0,213,</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="8"/>
+        <v>43,0,255,</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,213,</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="10"/>
+        <v>255,43,0,</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="11"/>
+        <v>213,255,0,</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,43,</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="13"/>
+        <v>0,213,255,</v>
+      </c>
+      <c r="K12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>16</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="7"/>
+        <v>255,0,191,</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="8"/>
+        <v>64,0,255,</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,191,</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="10"/>
+        <v>255,64,0,</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="11"/>
+        <v>191,255,0,</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,64,</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="13"/>
+        <v>0,191,255,</v>
+      </c>
+      <c r="K13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>29</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="7"/>
+        <v>255,85,0,</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="8"/>
+        <v>85,0,255,</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,170,</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="10"/>
+        <v>255,85,0,</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="11"/>
+        <v>170,255,0,</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,85,</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="13"/>
+        <v>0,170,255,</v>
+      </c>
+      <c r="K14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>28</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="7"/>
+        <v>255,106,0,</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="8"/>
+        <v>106,0,255,</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,149,</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="10"/>
+        <v>255,106,0,</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="11"/>
+        <v>149,255,0,</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,106,</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="13"/>
+        <v>0,149,255,</v>
+      </c>
+      <c r="K15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>27</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="7"/>
+        <v>128,255,0,</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="8"/>
+        <v>128,0,255,</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,128,</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="10"/>
+        <v>255,128,0,</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="11"/>
+        <v>128,255,0,</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,128,</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="13"/>
+        <v>0,128,255,</v>
+      </c>
+      <c r="K16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>26</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="7"/>
+        <v>106,255,0,</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="8"/>
+        <v>149,0,255,</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,106,</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="10"/>
+        <v>255,149,0,</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="11"/>
+        <v>106,255,0,</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,149,</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="13"/>
+        <v>0,106,255,</v>
+      </c>
+      <c r="K17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>25</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="7"/>
+        <v>0,255,170,</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="8"/>
+        <v>170,0,255,</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,85,</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="10"/>
+        <v>255,170,0,</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="11"/>
+        <v>85,255,0,</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,170,</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="13"/>
+        <v>0,85,255,</v>
+      </c>
+      <c r="K18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>22</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="7"/>
+        <v>0,255,191,</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="8"/>
+        <v>191,0,255,</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,64,</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="10"/>
+        <v>255,191,0,</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="11"/>
+        <v>64,255,0,</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,191,</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="13"/>
+        <v>0,64,255,</v>
+      </c>
+      <c r="K19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="7"/>
+        <v>0,43,255,</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="8"/>
+        <v>213,0,255,</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,43,</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="10"/>
+        <v>255,213,0,</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="11"/>
+        <v>43,255,0,</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,213,</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="13"/>
+        <v>0,43,255,</v>
+      </c>
+      <c r="K20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="7"/>
+        <v>0,21,255,</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="8"/>
+        <v>234,0,255,</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,21,</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="10"/>
+        <v>255,234,0,</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="11"/>
+        <v>21,255,0,</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,234,</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="13"/>
+        <v>0,21,255,</v>
+      </c>
+      <c r="K21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="7"/>
+        <v>0,0,255,</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="8"/>
+        <v>0,0,255,</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,255,</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="10"/>
+        <v>255,0,0,</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="11"/>
+        <v>255,255,0,</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,0,</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="13"/>
+        <v>0,255,255,</v>
+      </c>
+      <c r="K22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="7"/>
+        <v>17,0,255,</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="8"/>
+        <v>17,0,255,</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,238,</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="10"/>
+        <v>255,17,0,</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="11"/>
+        <v>238,255,0,</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,17,</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="13"/>
+        <v>0,238,255,</v>
+      </c>
+      <c r="K23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="7"/>
+        <v>34,0,255,</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="8"/>
+        <v>34,0,255,</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,221,</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="10"/>
+        <v>255,34,0,</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="11"/>
+        <v>221,255,0,</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,34,</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="13"/>
+        <v>0,221,255,</v>
+      </c>
+      <c r="K24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>14</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="7"/>
+        <v>255,0,204,</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="8"/>
+        <v>51,0,255,</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,204,</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="10"/>
+        <v>255,51,0,</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="11"/>
+        <v>204,255,0,</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,51,</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="13"/>
+        <v>0,204,255,</v>
+      </c>
+      <c r="K25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>15</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="7"/>
+        <v>255,0,187,</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="8"/>
+        <v>68,0,255,</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,187,</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="10"/>
+        <v>255,68,0,</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="11"/>
+        <v>187,255,0,</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,68,</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="13"/>
+        <v>0,187,255,</v>
+      </c>
+      <c r="K26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>30</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="7"/>
+        <v>255,85,0,</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="8"/>
+        <v>85,0,255,</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,170,</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="10"/>
+        <v>255,85,0,</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="11"/>
+        <v>170,255,0,</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,85,</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="13"/>
+        <v>0,170,255,</v>
+      </c>
+      <c r="K27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>31</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="7"/>
+        <v>255,102,0,</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="8"/>
+        <v>102,0,255,</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,153,</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="10"/>
+        <v>255,102,0,</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="11"/>
+        <v>153,255,0,</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,102,</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="13"/>
+        <v>0,153,255,</v>
+      </c>
+      <c r="K28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29">
+        <v>32</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="7"/>
+        <v>255,119,0,</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="8"/>
+        <v>119,0,255,</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,136,</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="10"/>
+        <v>255,119,0,</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="11"/>
+        <v>136,255,0,</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,119,</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="13"/>
+        <v>0,136,255,</v>
+      </c>
+      <c r="K29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>33</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="7"/>
+        <v>119,255,0,</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="8"/>
+        <v>136,0,255,</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,119,</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="10"/>
+        <v>255,136,0,</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="11"/>
+        <v>119,255,0,</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,136,</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="13"/>
+        <v>0,119,255,</v>
+      </c>
+      <c r="K30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>34</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="7"/>
+        <v>102,255,0,</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="8"/>
+        <v>153,0,255,</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,102,</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="10"/>
+        <v>255,153,0,</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="11"/>
+        <v>102,255,0,</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,153,</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="13"/>
+        <v>0,102,255,</v>
+      </c>
+      <c r="K31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>24</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="7"/>
+        <v>0,255,170,</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="8"/>
+        <v>170,0,255,</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,85,</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="10"/>
+        <v>255,170,0,</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="11"/>
+        <v>85,255,0,</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,170,</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="13"/>
+        <v>0,85,255,</v>
+      </c>
+      <c r="K32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>11</v>
+      </c>
+      <c r="B33">
+        <v>23</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="7"/>
+        <v>0,255,187,</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="8"/>
+        <v>187,0,255,</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,68,</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="10"/>
+        <v>255,187,0,</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="11"/>
+        <v>68,255,0,</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,187,</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="13"/>
+        <v>0,68,255,</v>
+      </c>
+      <c r="K33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>12</v>
+      </c>
+      <c r="B34">
+        <v>9</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="7"/>
+        <v>0,255,204,</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="8"/>
+        <v>204,0,255,</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,51,</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="10"/>
+        <v>255,204,0,</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="11"/>
+        <v>51,255,0,</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,204,</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="13"/>
+        <v>0,51,255,</v>
+      </c>
+      <c r="K34">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>13</v>
+      </c>
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="7"/>
+        <v>0,34,255,</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="8"/>
+        <v>221,0,255,</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,34,</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="10"/>
+        <v>255,221,0,</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="11"/>
+        <v>34,255,0,</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,221,</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="13"/>
+        <v>0,34,255,</v>
+      </c>
+      <c r="K35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="7"/>
+        <v>0,17,255,</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="8"/>
+        <v>238,0,255,</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="9"/>
+        <v>255,0,17,</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="10"/>
+        <v>255,238,0,</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="11"/>
+        <v>17,255,0,</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="12"/>
+        <v>0,255,238,</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="13"/>
+        <v>0,17,255,</v>
+      </c>
+      <c r="K36">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>